<commit_message>
fixed the location of some buttons
</commit_message>
<xml_diff>
--- a/ListOfCountries.xlsx
+++ b/ListOfCountries.xlsx
@@ -768,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,7 +974,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>9.75</v>
+        <v>8.5</v>
       </c>
       <c r="D9">
         <v>5.5</v>
@@ -1173,7 +1173,7 @@
         <v>20</v>
       </c>
       <c r="C17">
-        <v>2.75</v>
+        <v>1.75</v>
       </c>
       <c r="D17">
         <v>28.5</v>
@@ -1216,7 +1216,7 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>28.5</v>
@@ -1818,7 +1818,7 @@
         <v>25</v>
       </c>
       <c r="D44">
-        <v>27.75</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
some buttons and stuff
</commit_message>
<xml_diff>
--- a/ListOfCountries.xlsx
+++ b/ListOfCountries.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10608" windowHeight="7584"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11076" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -762,1266 +762,1466 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
-    <col min="11" max="11" width="19.109375" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.21875" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.77734375" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>6.5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
+        <f>B2+1</f>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2.5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>59</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B51" si="0">B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>6</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>7.5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>65</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>66</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1.5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>63</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>5.5</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>11.25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>69</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>70</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>66</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>71</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2.5</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>13.75</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>63</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>69</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>72</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>8.5</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>5.5</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>65</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>122</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>6.5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>67</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>68</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>72</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>3.5</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>18.5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>70</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>73</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>75</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>74</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>1.5</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>3</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>21.5</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>72</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>77</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>78</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>6.25</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>20.5</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>75</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>72</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>76</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>78</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>80</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>5.25</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>23.75</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>76</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>77</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>81</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>82</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>83</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>2.5</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>25</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>76</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>78</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>82</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>1.75</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>28.5</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>79</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>78</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>7.75</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>25</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>77</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>78</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>82</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>4.75</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>28.5</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>79</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>78</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>81</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>85</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>6</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>30.5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>82</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>55</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>13.5</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>16.5</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>87</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
         <v>25</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>13.25</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>20.5</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>77</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>81</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>89</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>87</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
         <v>91</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>15</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>19.25</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>89</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>88</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>90</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>17.25</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>20.25</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>87</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>90</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>93</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>19.75</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>20</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>96</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
         <v>26</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>15.25</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>25.75</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>88</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>87</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>92</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>93</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>98</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
         <v>27</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>14</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>29.5</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>85</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>100</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>56</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
         <v>29</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>19</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>24.75</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>90</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>92</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>94</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>96</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>101</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
         <v>30</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>18.5</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>29.25</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>86</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>90</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>93</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>101</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
         <v>31</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>21</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>27</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>98</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>93</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>96</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>103</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>104</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
         <v>32</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>21.5</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>29.75</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>98</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>101</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>104</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
         <v>33</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>23</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>33.5</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>101</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>103</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>105</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
         <v>34</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>22</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>37.5</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>102</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
         <v>35</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>22</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>17.5</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>94</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>96</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
         <v>36</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>23.25</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>23</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>94</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>97</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>106</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>107</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>103</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>101</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
         <v>37</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>25.5</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>18.75</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>97</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>96</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>107</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
         <v>108</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>26.5</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>24.75</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>96</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>109</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>110</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>111</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
         <v>38</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>28.75</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>19.5</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>112</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>113</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>110</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>107</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
         <v>39</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>31.5</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>23.5</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>109</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>113</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>114</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
         <v>111</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
         <v>40</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>31</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>16</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>115</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>113</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>109</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
         <v>41</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>32.25</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>19.5</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>109</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>112</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>115</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>114</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
         <v>42</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>36.700000000000003</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>16.5</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>113</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>112</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
         <v>43</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>32.799999999999997</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>8</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="1">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
         <v>44</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>24.25</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>27.75</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>101</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>96</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>107</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>111</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>117</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
         <v>45</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>28</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>30.25</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>103</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>111</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>118</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B46" s="1">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
         <v>46</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>31</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>28.75</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>103</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>107</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>110</v>
       </c>
-      <c r="H46" t="s">
+      <c r="I46" t="s">
         <v>114</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>120</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>121</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>118</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B47" t="s">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
         <v>47</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>34.75</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>24.75</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>110</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>113</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>120</v>
       </c>
-      <c r="H47" t="s">
+      <c r="I47" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
         <v>48</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>34.75</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>29.5</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>111</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>114</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>121</v>
       </c>
-      <c r="H48" t="s">
+      <c r="I48" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C49" t="s">
         <v>49</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>28.75</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>34.75</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>117</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
         <v>50</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>30.1</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>31.75</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>119</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>117</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>111</v>
       </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>120</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
         <v>51</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>34.35</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>32.75</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>118</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>130</v>
       </c>

</xml_diff>